<commit_message>
changed to new ArcGIS account
</commit_message>
<xml_diff>
--- a/excel_files/dol_table_file_mappings.xlsx
+++ b/excel_files/dol_table_file_mappings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexpiazza/Desktop/for_db/excel_files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://txriogrande-my.sharepoint.com/personal/eshackney_trla_org/Documents/Projects/Farmworker Data Project/H2Data backend/trla-H2Data-backend/excel_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D83D2701-5BF7-0C4D-B358-41953099517A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="13_ncr:1_{D83D2701-5BF7-0C4D-B358-41953099517A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{A3C3997E-3010-419F-8ACF-A9AE8FD3791C}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{42026151-3EC6-E74B-A357-F0243FFB0ADE}"/>
+    <workbookView xWindow="36570" yWindow="4935" windowWidth="8625" windowHeight="10500" xr2:uid="{42026151-3EC6-E74B-A357-F0243FFB0ADE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>file_name</t>
   </si>
@@ -42,46 +42,43 @@
     <t>table_name</t>
   </si>
   <si>
-    <t>H-2A_AddendumA_FY2020.xlsx</t>
-  </si>
-  <si>
     <t>h2a_addendum_a</t>
   </si>
   <si>
-    <t>H-2B_Foreign_Labor_Recruiter_List_FY2020.xlsx</t>
-  </si>
-  <si>
-    <t>h2b_foreign_labor_recruiters</t>
-  </si>
-  <si>
-    <t>H2B_AppendixA_FY2020.xlsx</t>
-  </si>
-  <si>
     <t>h2b_appendix_a</t>
   </si>
   <si>
-    <t>H2B_AppendixC_FY2020.xlsx</t>
-  </si>
-  <si>
     <t>h2b_appendix_c</t>
   </si>
   <si>
-    <t>H2B_AppendixD_FY2020.xlsx</t>
-  </si>
-  <si>
     <t>h2b_appendix_d</t>
   </si>
   <si>
-    <t>PW_Disclosure_Data_FY2020.xlsx</t>
-  </si>
-  <si>
     <t>pw_disclosure</t>
   </si>
   <si>
-    <t>PW_Worksites_FY2020.xlsx</t>
-  </si>
-  <si>
     <t>pw_worksites</t>
+  </si>
+  <si>
+    <t>H-2A_Addendum_A_Disclosure_Data_FY2021_Q2.xls</t>
+  </si>
+  <si>
+    <t>H-2B_Appendix_A_FY2021_Q2.xls</t>
+  </si>
+  <si>
+    <t>H-2B_Appendix_C_FY2021_Q2.xls</t>
+  </si>
+  <si>
+    <t>H-2B_Appendix_D_FY2021_Q2.xls</t>
+  </si>
+  <si>
+    <t>PW_Disclosure_Data_FY2021_Q2.xls</t>
+  </si>
+  <si>
+    <t>PW_Disclosure_Data_FY2021_Q2_2.xls</t>
+  </si>
+  <si>
+    <t>PW_Worksites_FY2021_Q2.xls</t>
   </si>
 </sst>
 </file>
@@ -436,16 +433,16 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="A2" sqref="A2:B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="44.6640625" customWidth="1"/>
     <col min="2" max="2" width="26" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -453,60 +450,60 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
         <v>6</v>
       </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update MOST_RECENT_RUN_URL and DATE_OF_RUN_URL in .env file for new Apify actor, and update files names for Q4 update
</commit_message>
<xml_diff>
--- a/excel_files/dol_table_file_mappings.xlsx
+++ b/excel_files/dol_table_file_mappings.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://txriogrande-my.sharepoint.com/personal/eshackney_trla_org/Documents/Projects/Farmworker Data Project/H2Data backend/trla-H2Data-backend/excel_files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://txriogrande-my.sharepoint.com/personal/anovak_trla_org/Documents/Projects/trla-H2Data-backend/excel_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="17" documentId="13_ncr:1_{D83D2701-5BF7-0C4D-B358-41953099517A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{A3C3997E-3010-419F-8ACF-A9AE8FD3791C}"/>
+  <xr:revisionPtr revIDLastSave="27" documentId="13_ncr:1_{D83D2701-5BF7-0C4D-B358-41953099517A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{05FE9052-48D6-46F1-BA53-0CA876CD5C9D}"/>
   <bookViews>
-    <workbookView xWindow="36570" yWindow="4935" windowWidth="8625" windowHeight="10500" xr2:uid="{42026151-3EC6-E74B-A357-F0243FFB0ADE}"/>
+    <workbookView xWindow="28950" yWindow="225" windowWidth="10455" windowHeight="15045" xr2:uid="{42026151-3EC6-E74B-A357-F0243FFB0ADE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>file_name</t>
   </si>
@@ -60,25 +60,28 @@
     <t>pw_worksites</t>
   </si>
   <si>
-    <t>H-2A_Addendum_A_Disclosure_Data_FY2021_Q2.xls</t>
-  </si>
-  <si>
-    <t>H-2B_Appendix_A_FY2021_Q2.xls</t>
-  </si>
-  <si>
-    <t>H-2B_Appendix_C_FY2021_Q2.xls</t>
-  </si>
-  <si>
-    <t>H-2B_Appendix_D_FY2021_Q2.xls</t>
-  </si>
-  <si>
-    <t>PW_Disclosure_Data_FY2021_Q2.xls</t>
-  </si>
-  <si>
-    <t>PW_Disclosure_Data_FY2021_Q2_2.xls</t>
-  </si>
-  <si>
-    <t>PW_Worksites_FY2021_Q2.xls</t>
+    <t>H-2A_Addendum_A_FY2021_Q3.xls</t>
+  </si>
+  <si>
+    <t>H-2B_Appendix_A_FY2021_Q3.xls</t>
+  </si>
+  <si>
+    <t>H-2B_Appendix_C_FY2021_Q3.xls</t>
+  </si>
+  <si>
+    <t>H-2B_Appendix_D_FY2021_Q3.xls</t>
+  </si>
+  <si>
+    <t>h2b_foreign_labor_recruiters</t>
+  </si>
+  <si>
+    <t>Foreign_Labor_Recruiter_list_FY2021_Q3.xls</t>
+  </si>
+  <si>
+    <t>PW_Disclosure_Data_FY2021_Q3_old_form.xls</t>
+  </si>
+  <si>
+    <t>PW_Worksites_FY2021_Q3_old_form.xls</t>
   </si>
 </sst>
 </file>
@@ -433,16 +436,16 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B8"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.69921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="44.6640625" customWidth="1"/>
+    <col min="1" max="1" width="45.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -450,7 +453,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -458,7 +461,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -466,7 +469,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -474,7 +477,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -482,25 +485,25 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
@@ -508,5 +511,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update column mappings for quarterly data merge and update database URL
</commit_message>
<xml_diff>
--- a/excel_files/dol_table_file_mappings.xlsx
+++ b/excel_files/dol_table_file_mappings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://txriogrande-my.sharepoint.com/personal/anovak_trla_org/Documents/Projects/trla-H2Data-backend/excel_files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://txriogrande-my.sharepoint.com/personal/anovak_trla_org/Documents/Farmworker Projects/trla-H2Data-backend/excel_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="27" documentId="13_ncr:1_{D83D2701-5BF7-0C4D-B358-41953099517A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{05FE9052-48D6-46F1-BA53-0CA876CD5C9D}"/>
+  <xr:revisionPtr revIDLastSave="29" documentId="13_ncr:1_{D83D2701-5BF7-0C4D-B358-41953099517A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{39F939AD-42A7-4799-981B-D165648CDE07}"/>
   <bookViews>
-    <workbookView xWindow="28950" yWindow="225" windowWidth="10455" windowHeight="15045" xr2:uid="{42026151-3EC6-E74B-A357-F0243FFB0ADE}"/>
+    <workbookView xWindow="35985" yWindow="2370" windowWidth="18585" windowHeight="13380" xr2:uid="{42026151-3EC6-E74B-A357-F0243FFB0ADE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>file_name</t>
   </si>
@@ -82,6 +82,15 @@
   </si>
   <si>
     <t>PW_Worksites_FY2021_Q3_old_form.xls</t>
+  </si>
+  <si>
+    <t>PW_Worksites_FY2022_Q1_revised_form_h2b.xlsx</t>
+  </si>
+  <si>
+    <t>pw_worksites_new</t>
+  </si>
+  <si>
+    <t>THIS IS A SAMPLE</t>
   </si>
 </sst>
 </file>
@@ -433,10 +442,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69F219B8-D6F3-C840-8795-12309BB3B924}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="A7" sqref="A2:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.69921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -509,6 +518,19 @@
         <v>7</v>
       </c>
     </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>